<commit_message>
"#56": Tests unitarios para importar/exportar grupos
Se han añadido tests para probar las funciones del archivo "import_and_export.py"
</commit_message>
<xml_diff>
--- a/decide/authentication/files/testfiles/testgroup1.xlsx
+++ b/decide/authentication/files/testfiles/testgroup1.xlsx
@@ -20,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t xml:space="preserve">username2</t>
+  </si>
   <si>
     <t xml:space="preserve">username5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username3</t>
   </si>
   <si>
     <t xml:space="preserve">username1</t>
   </si>
   <si>
-    <t xml:space="preserve">username2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username3</t>
+    <t xml:space="preserve">username4</t>
   </si>
 </sst>
 </file>
@@ -132,13 +135,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -160,6 +163,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Revert "Modificaciones según los comentarios de la revisión M2"
</commit_message>
<xml_diff>
--- a/decide/authentication/files/testfiles/testgroup1.xlsx
+++ b/decide/authentication/files/testfiles/testgroup1.xlsx
@@ -20,21 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">username2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">username5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username3</t>
   </si>
   <si>
     <t xml:space="preserve">username1</t>
   </si>
   <si>
-    <t xml:space="preserve">username4</t>
+    <t xml:space="preserve">username2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username3</t>
   </si>
 </sst>
 </file>
@@ -135,13 +132,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -163,11 +160,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>